<commit_message>
v 3.1.5 fixed icdcode I425 for hf
</commit_message>
<xml_diff>
--- a/metadata/meta_variables.xlsx
+++ b/metadata/meta_variables.xlsx
@@ -1011,9 +1011,6 @@
     <t>Also see sos_durationhf</t>
   </si>
   <si>
-    <t>ICD-codes see https://kiheartfailure.github.io/shfdb3/. Also see shf_durationhf</t>
-  </si>
-  <si>
     <t>ICD-codes see https://kiheartfailure.github.io/shfdb3/. Also see shf_diabetes</t>
   </si>
   <si>
@@ -1084,6 +1081,9 @@
   </si>
   <si>
     <t>shf_rasarni</t>
+  </si>
+  <si>
+    <t>ICD-codes see https://kiheartfailure.github.io/shfdb3/. Time since hosp/visit in any DIA position to shf_indexdtm. Also see shf_durationhf</t>
   </si>
 </sst>
 </file>
@@ -1463,8 +1463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="A116" sqref="A116:XFD116"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="E90" sqref="E90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1575,7 +1575,7 @@
         <v>302</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1589,12 +1589,12 @@
         <v>206</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>205</v>
@@ -1603,10 +1603,10 @@
         <v>206</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1647,7 +1647,7 @@
         <v>290</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1677,7 +1677,7 @@
         <v>203</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>329</v>
@@ -1807,7 +1807,7 @@
         <v>159</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>320</v>
@@ -2039,7 +2039,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>182</v>
@@ -2091,7 +2091,7 @@
         <v>186</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2105,7 +2105,7 @@
         <v>321</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>327</v>
@@ -2215,7 +2215,7 @@
         <v>227</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E68" s="4" t="s">
         <v>222</v>
@@ -2229,24 +2229,24 @@
         <v>193</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>193</v>
       </c>
       <c r="D70" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="E70" s="4" t="s">
         <v>349</v>
-      </c>
-      <c r="E70" s="4" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -2257,10 +2257,10 @@
         <v>194</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -2271,10 +2271,10 @@
         <v>228</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -2285,7 +2285,7 @@
         <v>229</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -2296,7 +2296,7 @@
         <v>230</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -2307,10 +2307,10 @@
         <v>231</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -2321,10 +2321,10 @@
         <v>195</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -2335,10 +2335,10 @@
         <v>224</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -2455,7 +2455,7 @@
         <v>203</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>330</v>
+        <v>354</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -2466,7 +2466,7 @@
         <v>194</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -2477,7 +2477,7 @@
         <v>193</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -2543,7 +2543,7 @@
         <v>231</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -2565,7 +2565,7 @@
         <v>228</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
mod vardesc a bit more...
</commit_message>
<xml_diff>
--- a/metadata/meta_variables.xlsx
+++ b/metadata/meta_variables.xlsx
@@ -711,9 +711,6 @@
     <t>Dilated cardiomyopathy</t>
   </si>
   <si>
-    <t>Chilren</t>
-  </si>
-  <si>
     <t>Region</t>
   </si>
   <si>
@@ -1084,6 +1081,9 @@
   </si>
   <si>
     <t>Obstructive sleep apnea</t>
+  </si>
+  <si>
+    <t>Children</t>
   </si>
 </sst>
 </file>
@@ -1463,8 +1463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1488,10 +1488,10 @@
         <v>153</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1499,7 +1499,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1507,7 +1507,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1523,7 +1523,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1531,7 +1531,7 @@
         <v>4</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1542,7 +1542,7 @@
         <v>194</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1558,7 +1558,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1572,10 +1572,10 @@
         <v>204</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1589,12 +1589,12 @@
         <v>204</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>203</v>
@@ -1603,10 +1603,10 @@
         <v>204</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1636,7 +1636,7 @@
         <v>200</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1644,10 +1644,10 @@
         <v>11</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1658,7 +1658,7 @@
         <v>198</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1677,10 +1677,10 @@
         <v>201</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1691,7 +1691,7 @@
         <v>202</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1699,7 +1699,7 @@
         <v>16</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1732,7 +1732,7 @@
         <v>163</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1807,10 +1807,10 @@
         <v>159</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1833,7 +1833,7 @@
         <v>166</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1844,7 +1844,7 @@
         <v>167</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D34" s="1"/>
     </row>
@@ -1856,7 +1856,7 @@
         <v>168</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1870,7 +1870,7 @@
         <v>204</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1881,10 +1881,10 @@
         <v>162</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1898,7 +1898,7 @@
         <v>213</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1906,10 +1906,10 @@
         <v>36</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1928,7 +1928,7 @@
         <v>171</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1939,10 +1939,10 @@
         <v>172</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1953,7 +1953,7 @@
         <v>173</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1980,10 +1980,10 @@
         <v>175</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -2010,10 +2010,10 @@
         <v>180</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -2024,28 +2024,28 @@
         <v>181</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E50" s="3"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="B51" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="B51" s="4" t="s">
-        <v>292</v>
-      </c>
       <c r="C51" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E51" s="3"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>182</v>
@@ -2075,10 +2075,10 @@
         <v>185</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -2097,7 +2097,7 @@
         <v>186</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2108,13 +2108,13 @@
         <v>187</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -2130,7 +2130,7 @@
         <v>53</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2138,10 +2138,10 @@
         <v>54</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -2165,13 +2165,13 @@
         <v>57</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -2179,16 +2179,16 @@
         <v>58</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C65" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="E65" s="4" t="s">
         <v>310</v>
-      </c>
-      <c r="D65" s="4" t="s">
-        <v>309</v>
-      </c>
-      <c r="E65" s="4" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -2196,13 +2196,13 @@
         <v>59</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -2221,7 +2221,7 @@
         <v>225</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E68" s="4" t="s">
         <v>220</v>
@@ -2235,24 +2235,24 @@
         <v>191</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>191</v>
       </c>
       <c r="D70" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="E70" s="4" t="s">
         <v>344</v>
-      </c>
-      <c r="E70" s="4" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -2263,10 +2263,10 @@
         <v>192</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -2277,10 +2277,10 @@
         <v>226</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -2291,7 +2291,7 @@
         <v>227</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -2302,7 +2302,7 @@
         <v>228</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -2313,10 +2313,10 @@
         <v>229</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -2327,10 +2327,10 @@
         <v>193</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -2341,10 +2341,10 @@
         <v>222</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -2352,10 +2352,10 @@
         <v>69</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -2363,7 +2363,7 @@
         <v>70</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -2371,7 +2371,7 @@
         <v>71</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -2379,7 +2379,7 @@
         <v>72</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -2387,10 +2387,10 @@
         <v>73</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>230</v>
+        <v>354</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -2398,7 +2398,7 @@
         <v>74</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -2406,7 +2406,7 @@
         <v>75</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -2414,10 +2414,10 @@
         <v>76</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -2425,10 +2425,10 @@
         <v>77</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -2450,7 +2450,7 @@
         <v>217</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -2461,7 +2461,7 @@
         <v>201</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -2472,7 +2472,7 @@
         <v>192</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -2483,7 +2483,7 @@
         <v>191</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -2491,10 +2491,10 @@
         <v>83</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -2502,10 +2502,10 @@
         <v>84</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -2513,10 +2513,10 @@
         <v>85</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E94" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -2524,10 +2524,10 @@
         <v>86</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E95" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -2535,10 +2535,10 @@
         <v>87</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E96" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -2549,7 +2549,7 @@
         <v>229</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -2557,10 +2557,10 @@
         <v>89</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E98" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -2571,7 +2571,7 @@
         <v>226</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -2579,10 +2579,10 @@
         <v>91</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E100" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2590,10 +2590,10 @@
         <v>92</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E101" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -2601,10 +2601,10 @@
         <v>93</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E102" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -2612,10 +2612,10 @@
         <v>94</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E103" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -2623,10 +2623,10 @@
         <v>95</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E104" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -2634,10 +2634,10 @@
         <v>96</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E105" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -2645,10 +2645,10 @@
         <v>97</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E106" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -2656,10 +2656,10 @@
         <v>98</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E107" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -2667,10 +2667,10 @@
         <v>99</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E108" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -2678,10 +2678,10 @@
         <v>100</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E109" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -2689,10 +2689,10 @@
         <v>101</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E110" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -2700,10 +2700,10 @@
         <v>102</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E111" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -2711,10 +2711,10 @@
         <v>103</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E112" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -2722,10 +2722,10 @@
         <v>104</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E113" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -2733,10 +2733,10 @@
         <v>105</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E114" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -2744,10 +2744,10 @@
         <v>106</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E115" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -2755,10 +2755,10 @@
         <v>107</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E116" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -2766,10 +2766,10 @@
         <v>108</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E117" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -2777,10 +2777,10 @@
         <v>109</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E118" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -2788,7 +2788,7 @@
         <v>110</v>
       </c>
       <c r="E119" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -2796,10 +2796,10 @@
         <v>111</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E120" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -2807,7 +2807,7 @@
         <v>112</v>
       </c>
       <c r="E121" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -2815,10 +2815,10 @@
         <v>113</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E122" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -2826,7 +2826,7 @@
         <v>114</v>
       </c>
       <c r="E123" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
@@ -2834,10 +2834,10 @@
         <v>115</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E124" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
@@ -2845,7 +2845,7 @@
         <v>116</v>
       </c>
       <c r="E125" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -2853,10 +2853,10 @@
         <v>117</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E126" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -2864,7 +2864,7 @@
         <v>118</v>
       </c>
       <c r="E127" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -2872,10 +2872,10 @@
         <v>119</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E128" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -2883,7 +2883,7 @@
         <v>120</v>
       </c>
       <c r="E129" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -2891,10 +2891,10 @@
         <v>121</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E130" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -2902,7 +2902,7 @@
         <v>122</v>
       </c>
       <c r="E131" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -2910,10 +2910,10 @@
         <v>123</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E132" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -2921,7 +2921,7 @@
         <v>124</v>
       </c>
       <c r="E133" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -2929,7 +2929,7 @@
         <v>125</v>
       </c>
       <c r="E134" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -2937,10 +2937,10 @@
         <v>126</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E135" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -2948,7 +2948,7 @@
         <v>127</v>
       </c>
       <c r="E136" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -2956,10 +2956,10 @@
         <v>128</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E137" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -2967,7 +2967,7 @@
         <v>129</v>
       </c>
       <c r="E138" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -2975,10 +2975,10 @@
         <v>130</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E139" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -2986,7 +2986,7 @@
         <v>131</v>
       </c>
       <c r="E140" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -2994,10 +2994,10 @@
         <v>132</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E141" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -3005,7 +3005,7 @@
         <v>133</v>
       </c>
       <c r="E142" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -3013,10 +3013,10 @@
         <v>134</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E143" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -3024,7 +3024,7 @@
         <v>135</v>
       </c>
       <c r="E144" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -3032,10 +3032,10 @@
         <v>136</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E145" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -3043,7 +3043,7 @@
         <v>137</v>
       </c>
       <c r="E146" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -3051,10 +3051,10 @@
         <v>138</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E147" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
@@ -3062,7 +3062,7 @@
         <v>139</v>
       </c>
       <c r="E148" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -3070,10 +3070,10 @@
         <v>140</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E149" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
@@ -3081,7 +3081,7 @@
         <v>141</v>
       </c>
       <c r="E150" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -3089,10 +3089,10 @@
         <v>142</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E151" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -3100,7 +3100,7 @@
         <v>143</v>
       </c>
       <c r="E152" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -3108,10 +3108,10 @@
         <v>144</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E153" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -3119,7 +3119,7 @@
         <v>145</v>
       </c>
       <c r="E154" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -3127,10 +3127,10 @@
         <v>146</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E155" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -3138,7 +3138,7 @@
         <v>147</v>
       </c>
       <c r="E156" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -3146,10 +3146,10 @@
         <v>148</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E157" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
@@ -3157,10 +3157,10 @@
         <v>149</v>
       </c>
       <c r="B158" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E158" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -3168,10 +3168,10 @@
         <v>150</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E159" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -3179,12 +3179,12 @@
         <v>151</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v 3.1.7 tia and ntprobnp
</commit_message>
<xml_diff>
--- a/metadata/meta_variables.xlsx
+++ b/metadata/meta_variables.xlsx
@@ -114,9 +114,6 @@
     <t>shf_gfrckdepi</t>
   </si>
   <si>
-    <t>shf_ntpropbnp</t>
-  </si>
-  <si>
     <t>shf_bnp</t>
   </si>
   <si>
@@ -1090,6 +1087,9 @@
   </si>
   <si>
     <t>Centre type</t>
+  </si>
+  <si>
+    <t>shf_ntprobnp</t>
   </si>
 </sst>
 </file>
@@ -1470,7 +1470,7 @@
   <dimension ref="A1:E163"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1485,19 +1485,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>153</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1505,7 +1505,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1513,7 +1513,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1521,7 +1521,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1529,7 +1529,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1537,7 +1537,7 @@
         <v>4</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1545,10 +1545,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1556,7 +1556,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1564,7 +1564,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1572,16 +1572,16 @@
         <v>17</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>204</v>
-      </c>
       <c r="D10" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1589,30 +1589,30 @@
         <v>18</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>204</v>
-      </c>
       <c r="E11" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>340</v>
-      </c>
       <c r="E12" s="4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1620,7 +1620,7 @@
         <v>7</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1628,10 +1628,10 @@
         <v>9</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1639,10 +1639,10 @@
         <v>10</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1650,10 +1650,10 @@
         <v>11</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1661,18 +1661,18 @@
         <v>12</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>355</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1680,7 +1680,7 @@
         <v>13</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1688,13 +1688,13 @@
         <v>14</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1702,10 +1702,10 @@
         <v>15</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1713,7 +1713,7 @@
         <v>16</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1721,10 +1721,10 @@
         <v>19</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1732,10 +1732,10 @@
         <v>20</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1743,10 +1743,10 @@
         <v>21</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1754,10 +1754,10 @@
         <v>22</v>
       </c>
       <c r="B26" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>206</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1765,10 +1765,10 @@
         <v>23</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1776,7 +1776,7 @@
         <v>24</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1784,10 +1784,10 @@
         <v>25</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1795,10 +1795,10 @@
         <v>26</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1806,10 +1806,10 @@
         <v>27</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D31" s="1"/>
     </row>
@@ -1818,13 +1818,13 @@
         <v>28</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1832,10 +1832,10 @@
         <v>29</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D33" s="1"/>
     </row>
@@ -1844,1361 +1844,1361 @@
         <v>30</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>31</v>
+        <v>356</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D35" s="1"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E51" s="3"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="B52" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="B52" s="4" t="s">
-        <v>291</v>
-      </c>
       <c r="C52" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E52" s="3"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C66" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="E66" s="4" t="s">
         <v>309</v>
-      </c>
-      <c r="D66" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="E66" s="4" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D71" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="E71" s="4" t="s">
         <v>343</v>
-      </c>
-      <c r="E71" s="4" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E94" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E95" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E96" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E98" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E100" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E101" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E102" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E103" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E104" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E105" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E106" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E107" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E108" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E109" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E110" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E111" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E112" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E113" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E114" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E115" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E116" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E117" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E118" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E119" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E120" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E121" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E122" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E123" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E124" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E125" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E126" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E127" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E128" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E129" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E130" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E131" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E132" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E133" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E134" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E135" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E136" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E137" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E138" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E139" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E140" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E141" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E142" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E143" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E144" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E145" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E146" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E147" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E148" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E149" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B150" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E150" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E151" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E152" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E153" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E154" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E155" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E156" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E157" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B158" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E158" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E159" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E160" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B161" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v 3.3.3 sos_com_cancer3y only HDIA
</commit_message>
<xml_diff>
--- a/metadata/meta_variables.xlsx
+++ b/metadata/meta_variables.xlsx
@@ -1104,9 +1104,6 @@
     <t>Time since last HF hospitalization</t>
   </si>
   <si>
-    <t>ICD-codes see https://kiheartfailure.github.io/shfdb3/. Time since hosp (date of discharge (in-pat)/visit date (out-pat)) in any HDIA position to shf_indexdtm. Note that dates in NPR and SwedeHF can differ slightly so caution should be used when looking at small durations</t>
-  </si>
-  <si>
     <t>shf_indexhosptime</t>
   </si>
   <si>
@@ -1114,6 +1111,9 @@
   </si>
   <si>
     <t>days</t>
+  </si>
+  <si>
+    <t>ICD-codes see https://kiheartfailure.github.io/shfdb3/. Time since hosp (date of discharge) in any HDIA position to shf_indexdtm. Note that dates in NPR and SwedeHF can differ slightly so caution should be used when looking at small durations</t>
   </si>
 </sst>
 </file>
@@ -1493,8 +1493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD166"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="E93" sqref="E93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1577,13 +1577,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>363</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -18900,7 +18900,7 @@
         <v>200</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E92" s="4" t="s">
         <v>358</v>
@@ -18914,10 +18914,10 @@
         <v>360</v>
       </c>
       <c r="C93" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="E93" s="4" t="s">
         <v>364</v>
-      </c>
-      <c r="E93" s="4" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="94" spans="1:16384" x14ac:dyDescent="0.25">
@@ -19244,7 +19244,7 @@
         <v>109</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E123" s="4" t="s">
         <v>322</v>
@@ -19266,7 +19266,7 @@
         <v>111</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E125" s="4" t="s">
         <v>322</v>
@@ -19288,7 +19288,7 @@
         <v>113</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E127" s="4" t="s">
         <v>322</v>
@@ -19310,7 +19310,7 @@
         <v>115</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E129" s="4" t="s">
         <v>322</v>
@@ -19332,7 +19332,7 @@
         <v>117</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E131" s="4" t="s">
         <v>322</v>
@@ -19354,7 +19354,7 @@
         <v>119</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E133" s="4" t="s">
         <v>322</v>
@@ -19376,7 +19376,7 @@
         <v>121</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E135" s="4" t="s">
         <v>322</v>
@@ -19398,7 +19398,7 @@
         <v>123</v>
       </c>
       <c r="C137" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E137" s="4" t="s">
         <v>322</v>
@@ -19409,7 +19409,7 @@
         <v>124</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E138" s="4" t="s">
         <v>322</v>
@@ -19431,7 +19431,7 @@
         <v>126</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E140" s="4" t="s">
         <v>322</v>
@@ -19453,7 +19453,7 @@
         <v>128</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E142" s="4" t="s">
         <v>322</v>
@@ -19475,7 +19475,7 @@
         <v>130</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E144" s="4" t="s">
         <v>322</v>
@@ -19497,7 +19497,7 @@
         <v>132</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E146" s="4" t="s">
         <v>322</v>
@@ -19519,7 +19519,7 @@
         <v>134</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E148" s="4" t="s">
         <v>322</v>
@@ -19541,7 +19541,7 @@
         <v>136</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E150" s="4" t="s">
         <v>322</v>
@@ -19563,7 +19563,7 @@
         <v>138</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E152" s="4" t="s">
         <v>322</v>
@@ -19585,7 +19585,7 @@
         <v>140</v>
       </c>
       <c r="C154" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E154" s="4" t="s">
         <v>322</v>
@@ -19607,7 +19607,7 @@
         <v>142</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E156" s="4" t="s">
         <v>322</v>
@@ -19629,7 +19629,7 @@
         <v>144</v>
       </c>
       <c r="C158" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E158" s="4" t="s">
         <v>322</v>
@@ -19651,7 +19651,7 @@
         <v>146</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E160" s="4" t="s">
         <v>322</v>

</xml_diff>

<commit_message>
add info about prop hf hosp for shf_location
</commit_message>
<xml_diff>
--- a/metadata/meta_variables.xlsx
+++ b/metadata/meta_variables.xlsx
@@ -900,9 +900,6 @@
     <t>For internal use. If it is a post registred in the old or new (prior to April 2017) SwedeHF. Most index posts in old SwedeHF were migrated to new SwedeHF (New SHF migrated from old SHF)</t>
   </si>
   <si>
-    <t>For shf_source = New SHF &amp; shf_type = Follow-up Out-patient can include telephone or survey</t>
-  </si>
-  <si>
     <t>valid</t>
   </si>
   <si>
@@ -1114,6 +1111,9 @@
   </si>
   <si>
     <t>ICD-codes see https://kiheartfailure.github.io/shfdb3/. Time since hosp (date of discharge) in any HDIA position to shf_indexdtm. Note that dates in NPR and SwedeHF can differ slightly so caution should be used when looking at small durations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For shf_source = New SHF &amp; shf_type = Follow-up Out-patient can include telephone or survey. Of the in-patients approximately 2/3 have a corresponding hospitalization in the NPR with HF as main diagnosis. </t>
   </si>
 </sst>
 </file>
@@ -1493,8 +1493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E93" sqref="E93"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1518,7 +1518,7 @@
         <v>152</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>281</v>
@@ -1577,13 +1577,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>362</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1613,10 +1613,10 @@
         <v>203</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1630,12 +1630,12 @@
         <v>203</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>202</v>
@@ -1644,10 +1644,10 @@
         <v>203</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1677,7 +1677,7 @@
         <v>199</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1688,7 +1688,7 @@
         <v>284</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1699,15 +1699,15 @@
         <v>197</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>293</v>
+        <v>364</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>353</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1726,10 +1726,10 @@
         <v>200</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1740,7 +1740,7 @@
         <v>201</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1748,7 +1748,7 @@
         <v>16</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1781,7 +1781,7 @@
         <v>162</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1856,10 +1856,10 @@
         <v>158</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1882,18 +1882,18 @@
         <v>165</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>166</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D36" s="1"/>
     </row>
@@ -1905,7 +1905,7 @@
         <v>167</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1919,7 +1919,7 @@
         <v>203</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1930,10 +1930,10 @@
         <v>161</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1947,7 +1947,7 @@
         <v>212</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1958,7 +1958,7 @@
         <v>283</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1977,7 +1977,7 @@
         <v>170</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1988,10 +1988,10 @@
         <v>171</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -2002,7 +2002,7 @@
         <v>172</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -2029,10 +2029,10 @@
         <v>174</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -2059,10 +2059,10 @@
         <v>179</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -2073,7 +2073,7 @@
         <v>180</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E52" s="3"/>
     </row>
@@ -2085,16 +2085,16 @@
         <v>290</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E53" s="3"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>181</v>
@@ -2124,10 +2124,10 @@
         <v>184</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2146,7 +2146,7 @@
         <v>185</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2157,13 +2157,13 @@
         <v>186</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2179,7 +2179,7 @@
         <v>52</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -2187,10 +2187,10 @@
         <v>53</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -2214,13 +2214,13 @@
         <v>56</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -2228,16 +2228,16 @@
         <v>57</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C67" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="E67" s="4" t="s">
         <v>308</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="E67" s="4" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -2245,13 +2245,13 @@
         <v>58</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -2270,7 +2270,7 @@
         <v>224</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E70" s="4" t="s">
         <v>219</v>
@@ -2284,24 +2284,24 @@
         <v>190</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>190</v>
       </c>
       <c r="D72" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="E72" s="4" t="s">
         <v>342</v>
-      </c>
-      <c r="E72" s="4" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -2312,10 +2312,10 @@
         <v>191</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -2326,10 +2326,10 @@
         <v>225</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -2340,7 +2340,7 @@
         <v>226</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -2351,7 +2351,7 @@
         <v>227</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -2362,10 +2362,10 @@
         <v>228</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -2376,10 +2376,10 @@
         <v>192</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -2390,10 +2390,10 @@
         <v>221</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -2404,7 +2404,7 @@
         <v>282</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="81" spans="1:16384" x14ac:dyDescent="0.25">
@@ -2436,10 +2436,10 @@
         <v>72</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="85" spans="1:16384" x14ac:dyDescent="0.25">
@@ -2466,7 +2466,7 @@
         <v>232</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="88" spans="1:16384" x14ac:dyDescent="0.25">
@@ -2477,7 +2477,7 @@
         <v>230</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="89" spans="1:16384" x14ac:dyDescent="0.25">
@@ -2499,15 +2499,15 @@
         <v>216</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="91" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>355</v>
+      </c>
+      <c r="B91" s="4" t="s">
         <v>356</v>
-      </c>
-      <c r="B91" s="4" t="s">
-        <v>357</v>
       </c>
       <c r="C91"/>
       <c r="D91"/>
@@ -18900,24 +18900,24 @@
         <v>200</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="93" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="B93" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="B93" s="4" t="s">
-        <v>360</v>
-      </c>
       <c r="C93" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="E93" s="4" t="s">
         <v>363</v>
-      </c>
-      <c r="E93" s="4" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="94" spans="1:16384" x14ac:dyDescent="0.25">
@@ -18928,7 +18928,7 @@
         <v>191</v>
       </c>
       <c r="E94" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="95" spans="1:16384" x14ac:dyDescent="0.25">
@@ -18939,7 +18939,7 @@
         <v>190</v>
       </c>
       <c r="E95" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="96" spans="1:16384" x14ac:dyDescent="0.25">
@@ -18950,7 +18950,7 @@
         <v>236</v>
       </c>
       <c r="E96" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -18961,7 +18961,7 @@
         <v>237</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -18972,7 +18972,7 @@
         <v>238</v>
       </c>
       <c r="E98" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -18983,7 +18983,7 @@
         <v>239</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -18994,7 +18994,7 @@
         <v>240</v>
       </c>
       <c r="E100" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -19005,7 +19005,7 @@
         <v>228</v>
       </c>
       <c r="E101" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -19016,7 +19016,7 @@
         <v>241</v>
       </c>
       <c r="E102" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -19027,7 +19027,7 @@
         <v>225</v>
       </c>
       <c r="E103" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -19038,7 +19038,7 @@
         <v>242</v>
       </c>
       <c r="E104" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -19049,7 +19049,7 @@
         <v>243</v>
       </c>
       <c r="E105" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -19060,7 +19060,7 @@
         <v>244</v>
       </c>
       <c r="E106" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -19071,7 +19071,7 @@
         <v>245</v>
       </c>
       <c r="E107" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -19079,10 +19079,10 @@
         <v>94</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E108" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -19093,7 +19093,7 @@
         <v>246</v>
       </c>
       <c r="E109" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -19104,7 +19104,7 @@
         <v>247</v>
       </c>
       <c r="E110" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -19115,7 +19115,7 @@
         <v>248</v>
       </c>
       <c r="E111" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -19126,7 +19126,7 @@
         <v>249</v>
       </c>
       <c r="E112" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -19137,7 +19137,7 @@
         <v>250</v>
       </c>
       <c r="E113" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -19145,10 +19145,10 @@
         <v>100</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E114" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -19159,7 +19159,7 @@
         <v>251</v>
       </c>
       <c r="E115" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -19170,7 +19170,7 @@
         <v>252</v>
       </c>
       <c r="E116" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -19181,7 +19181,7 @@
         <v>253</v>
       </c>
       <c r="E117" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -19192,7 +19192,7 @@
         <v>254</v>
       </c>
       <c r="E118" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -19203,7 +19203,7 @@
         <v>255</v>
       </c>
       <c r="E119" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -19214,7 +19214,7 @@
         <v>256</v>
       </c>
       <c r="E120" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -19225,7 +19225,7 @@
         <v>258</v>
       </c>
       <c r="E121" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -19236,7 +19236,7 @@
         <v>259</v>
       </c>
       <c r="E122" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -19244,10 +19244,10 @@
         <v>109</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E123" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
@@ -19258,7 +19258,7 @@
         <v>260</v>
       </c>
       <c r="E124" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
@@ -19266,10 +19266,10 @@
         <v>111</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E125" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -19280,7 +19280,7 @@
         <v>262</v>
       </c>
       <c r="E126" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -19288,10 +19288,10 @@
         <v>113</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E127" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -19302,7 +19302,7 @@
         <v>263</v>
       </c>
       <c r="E128" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -19310,10 +19310,10 @@
         <v>115</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E129" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -19324,7 +19324,7 @@
         <v>264</v>
       </c>
       <c r="E130" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -19332,10 +19332,10 @@
         <v>117</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E131" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -19346,7 +19346,7 @@
         <v>265</v>
       </c>
       <c r="E132" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -19354,10 +19354,10 @@
         <v>119</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E133" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -19368,7 +19368,7 @@
         <v>266</v>
       </c>
       <c r="E134" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -19376,10 +19376,10 @@
         <v>121</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E135" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -19390,7 +19390,7 @@
         <v>267</v>
       </c>
       <c r="E136" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -19398,10 +19398,10 @@
         <v>123</v>
       </c>
       <c r="C137" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E137" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -19409,10 +19409,10 @@
         <v>124</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E138" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -19423,7 +19423,7 @@
         <v>268</v>
       </c>
       <c r="E139" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -19431,10 +19431,10 @@
         <v>126</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E140" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -19445,7 +19445,7 @@
         <v>261</v>
       </c>
       <c r="E141" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -19453,10 +19453,10 @@
         <v>128</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E142" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -19467,7 +19467,7 @@
         <v>269</v>
       </c>
       <c r="E143" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -19475,10 +19475,10 @@
         <v>130</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E144" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -19489,7 +19489,7 @@
         <v>271</v>
       </c>
       <c r="E145" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -19497,10 +19497,10 @@
         <v>132</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E146" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -19511,7 +19511,7 @@
         <v>270</v>
       </c>
       <c r="E147" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
@@ -19519,10 +19519,10 @@
         <v>134</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E148" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -19533,7 +19533,7 @@
         <v>273</v>
       </c>
       <c r="E149" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
@@ -19541,10 +19541,10 @@
         <v>136</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E150" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -19555,7 +19555,7 @@
         <v>274</v>
       </c>
       <c r="E151" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -19563,10 +19563,10 @@
         <v>138</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E152" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -19577,7 +19577,7 @@
         <v>275</v>
       </c>
       <c r="E153" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -19585,10 +19585,10 @@
         <v>140</v>
       </c>
       <c r="C154" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E154" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -19599,7 +19599,7 @@
         <v>276</v>
       </c>
       <c r="E155" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -19607,10 +19607,10 @@
         <v>142</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E156" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -19621,7 +19621,7 @@
         <v>277</v>
       </c>
       <c r="E157" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
@@ -19629,10 +19629,10 @@
         <v>144</v>
       </c>
       <c r="C158" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E158" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -19643,7 +19643,7 @@
         <v>272</v>
       </c>
       <c r="E159" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -19651,10 +19651,10 @@
         <v>146</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E160" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -19665,7 +19665,7 @@
         <v>278</v>
       </c>
       <c r="E161" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -19676,7 +19676,7 @@
         <v>279</v>
       </c>
       <c r="E162" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
@@ -19687,7 +19687,7 @@
         <v>257</v>
       </c>
       <c r="E163" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -19700,7 +19700,7 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="7" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change eGFR formula to 2021 v2.4.5
</commit_message>
<xml_diff>
--- a/metadata/meta_variables.xlsx
+++ b/metadata/meta_variables.xlsx
@@ -516,9 +516,6 @@
     <t>Heart rate</t>
   </si>
   <si>
-    <t>eGFR (CKD-EPI)</t>
-  </si>
-  <si>
     <t>NT-proBNP</t>
   </si>
   <si>
@@ -1120,6 +1117,9 @@
   </si>
   <si>
     <t>Derived from main position in NPR. Also see shf_location</t>
+  </si>
+  <si>
+    <t>eGFR (CKD-EPI 2021)</t>
   </si>
 </sst>
 </file>
@@ -1499,8 +1499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="E95" sqref="E95"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1524,10 +1524,10 @@
         <v>152</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1535,7 +1535,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1543,7 +1543,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1551,7 +1551,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1559,7 +1559,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1567,7 +1567,7 @@
         <v>4</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1575,21 +1575,21 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>361</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1597,7 +1597,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1605,7 +1605,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1613,16 +1613,16 @@
         <v>17</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>203</v>
-      </c>
       <c r="D11" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1630,30 +1630,30 @@
         <v>18</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>203</v>
-      </c>
       <c r="E12" s="4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>338</v>
-      </c>
       <c r="E13" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1661,7 +1661,7 @@
         <v>7</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1669,10 +1669,10 @@
         <v>9</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1680,10 +1680,10 @@
         <v>10</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1691,10 +1691,10 @@
         <v>11</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1702,18 +1702,18 @@
         <v>12</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>352</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1721,7 +1721,7 @@
         <v>13</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1729,13 +1729,13 @@
         <v>14</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1743,10 +1743,10 @@
         <v>15</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1754,7 +1754,7 @@
         <v>16</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1765,7 +1765,7 @@
         <v>154</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1776,7 +1776,7 @@
         <v>155</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1787,7 +1787,7 @@
         <v>162</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1795,10 +1795,10 @@
         <v>22</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>205</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1806,10 +1806,10 @@
         <v>23</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1828,7 +1828,7 @@
         <v>164</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1839,7 +1839,7 @@
         <v>156</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1850,7 +1850,7 @@
         <v>157</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D32" s="1"/>
     </row>
@@ -1862,10 +1862,10 @@
         <v>158</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1876,7 +1876,7 @@
         <v>159</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D34" s="1"/>
     </row>
@@ -1885,21 +1885,21 @@
         <v>30</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>165</v>
+        <v>366</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D36" s="1"/>
     </row>
@@ -1908,10 +1908,10 @@
         <v>31</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1922,10 +1922,10 @@
         <v>160</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1936,10 +1936,10 @@
         <v>161</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1947,13 +1947,13 @@
         <v>34</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1961,29 +1961,29 @@
         <v>35</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1991,13 +1991,13 @@
         <v>36</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -2005,10 +2005,10 @@
         <v>37</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -2016,7 +2016,7 @@
         <v>38</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -2024,7 +2024,7 @@
         <v>39</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -2032,13 +2032,13 @@
         <v>40</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -2046,7 +2046,7 @@
         <v>41</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -2054,7 +2054,7 @@
         <v>42</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -2062,13 +2062,13 @@
         <v>43</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -2076,34 +2076,34 @@
         <v>44</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E52" s="3"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="B53" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="B53" s="4" t="s">
-        <v>290</v>
-      </c>
       <c r="C53" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E53" s="3"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -2111,7 +2111,7 @@
         <v>45</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -2119,7 +2119,7 @@
         <v>46</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -2127,13 +2127,13 @@
         <v>47</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2141,7 +2141,7 @@
         <v>48</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -2149,10 +2149,10 @@
         <v>49</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2160,16 +2160,16 @@
         <v>50</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2177,7 +2177,7 @@
         <v>51</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -2185,7 +2185,7 @@
         <v>52</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -2193,10 +2193,10 @@
         <v>53</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -2204,7 +2204,7 @@
         <v>54</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -2212,7 +2212,7 @@
         <v>55</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -2220,13 +2220,13 @@
         <v>56</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -2234,16 +2234,16 @@
         <v>57</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C67" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="E67" s="4" t="s">
         <v>307</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="E67" s="4" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -2251,13 +2251,13 @@
         <v>58</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -2265,7 +2265,7 @@
         <v>59</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -2273,13 +2273,13 @@
         <v>60</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -2287,27 +2287,27 @@
         <v>61</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D72" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="E72" s="4" t="s">
         <v>341</v>
-      </c>
-      <c r="E72" s="4" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -2315,13 +2315,13 @@
         <v>62</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -2329,13 +2329,13 @@
         <v>63</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -2343,10 +2343,10 @@
         <v>64</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -2354,10 +2354,10 @@
         <v>65</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -2365,27 +2365,27 @@
         <v>66</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -2393,13 +2393,13 @@
         <v>67</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -2407,10 +2407,10 @@
         <v>68</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="81" spans="1:16384" x14ac:dyDescent="0.25">
@@ -2418,7 +2418,7 @@
         <v>69</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="82" spans="1:16384" x14ac:dyDescent="0.25">
@@ -2426,7 +2426,7 @@
         <v>70</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="83" spans="1:16384" x14ac:dyDescent="0.25">
@@ -2434,7 +2434,7 @@
         <v>71</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="84" spans="1:16384" x14ac:dyDescent="0.25">
@@ -2442,10 +2442,10 @@
         <v>72</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="85" spans="1:16384" x14ac:dyDescent="0.25">
@@ -2453,7 +2453,7 @@
         <v>73</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="86" spans="1:16384" x14ac:dyDescent="0.25">
@@ -2461,7 +2461,7 @@
         <v>74</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="87" spans="1:16384" x14ac:dyDescent="0.25">
@@ -2469,10 +2469,10 @@
         <v>75</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="88" spans="1:16384" x14ac:dyDescent="0.25">
@@ -2480,10 +2480,10 @@
         <v>76</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="89" spans="1:16384" x14ac:dyDescent="0.25">
@@ -2491,10 +2491,10 @@
         <v>77</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="90" spans="1:16384" x14ac:dyDescent="0.25">
@@ -2502,18 +2502,18 @@
         <v>78</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="91" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>354</v>
+      </c>
+      <c r="B91" s="4" t="s">
         <v>355</v>
-      </c>
-      <c r="B91" s="4" t="s">
-        <v>356</v>
       </c>
       <c r="C91"/>
       <c r="D91"/>
@@ -18903,38 +18903,38 @@
         <v>79</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="93" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="B93" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="B93" s="4" t="s">
-        <v>359</v>
-      </c>
       <c r="C93" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="E93" s="4" t="s">
         <v>362</v>
-      </c>
-      <c r="E93" s="4" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="94" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="E94" s="4" t="s">
         <v>365</v>
-      </c>
-      <c r="B94" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="E94" s="4" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="95" spans="1:16384" x14ac:dyDescent="0.25">
@@ -18942,10 +18942,10 @@
         <v>80</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E95" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="96" spans="1:16384" x14ac:dyDescent="0.25">
@@ -18953,10 +18953,10 @@
         <v>81</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E96" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -18964,10 +18964,10 @@
         <v>82</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -18975,10 +18975,10 @@
         <v>83</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E98" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -18986,10 +18986,10 @@
         <v>84</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -18997,10 +18997,10 @@
         <v>85</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E100" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -19008,10 +19008,10 @@
         <v>86</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E101" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -19019,10 +19019,10 @@
         <v>87</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E102" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -19030,10 +19030,10 @@
         <v>88</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E103" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -19041,10 +19041,10 @@
         <v>89</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E104" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -19052,10 +19052,10 @@
         <v>90</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E105" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -19063,10 +19063,10 @@
         <v>91</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E106" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -19074,10 +19074,10 @@
         <v>92</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E107" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -19085,10 +19085,10 @@
         <v>93</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E108" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -19096,10 +19096,10 @@
         <v>94</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E109" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -19107,10 +19107,10 @@
         <v>95</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E110" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -19118,10 +19118,10 @@
         <v>96</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E111" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -19129,10 +19129,10 @@
         <v>97</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E112" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -19140,10 +19140,10 @@
         <v>98</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E113" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -19151,10 +19151,10 @@
         <v>99</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E114" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -19162,10 +19162,10 @@
         <v>100</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E115" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -19173,10 +19173,10 @@
         <v>101</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E116" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -19184,10 +19184,10 @@
         <v>102</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E117" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -19195,10 +19195,10 @@
         <v>103</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E118" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -19206,10 +19206,10 @@
         <v>104</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E119" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -19217,10 +19217,10 @@
         <v>105</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E120" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -19228,10 +19228,10 @@
         <v>106</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E121" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -19239,10 +19239,10 @@
         <v>107</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E122" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -19250,10 +19250,10 @@
         <v>108</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E123" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
@@ -19261,10 +19261,10 @@
         <v>109</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E124" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
@@ -19272,10 +19272,10 @@
         <v>110</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E125" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -19283,10 +19283,10 @@
         <v>111</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E126" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -19294,10 +19294,10 @@
         <v>112</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E127" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -19305,10 +19305,10 @@
         <v>113</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E128" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -19316,10 +19316,10 @@
         <v>114</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E129" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -19327,10 +19327,10 @@
         <v>115</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E130" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -19338,10 +19338,10 @@
         <v>116</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E131" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -19349,10 +19349,10 @@
         <v>117</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E132" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -19360,10 +19360,10 @@
         <v>118</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E133" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -19371,10 +19371,10 @@
         <v>119</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E134" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -19382,10 +19382,10 @@
         <v>120</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E135" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -19393,10 +19393,10 @@
         <v>121</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E136" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -19404,10 +19404,10 @@
         <v>122</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E137" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -19415,10 +19415,10 @@
         <v>123</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E138" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -19426,10 +19426,10 @@
         <v>124</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E139" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -19437,10 +19437,10 @@
         <v>125</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E140" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -19448,10 +19448,10 @@
         <v>126</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E141" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -19459,10 +19459,10 @@
         <v>127</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E142" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -19470,10 +19470,10 @@
         <v>128</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E143" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -19481,10 +19481,10 @@
         <v>129</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E144" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -19492,10 +19492,10 @@
         <v>130</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E145" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -19503,10 +19503,10 @@
         <v>131</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E146" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -19514,10 +19514,10 @@
         <v>132</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E147" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
@@ -19525,10 +19525,10 @@
         <v>133</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E148" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -19536,10 +19536,10 @@
         <v>134</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E149" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
@@ -19547,10 +19547,10 @@
         <v>135</v>
       </c>
       <c r="B150" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E150" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -19558,10 +19558,10 @@
         <v>136</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E151" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -19569,10 +19569,10 @@
         <v>137</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E152" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -19580,10 +19580,10 @@
         <v>138</v>
       </c>
       <c r="C153" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E153" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -19591,10 +19591,10 @@
         <v>139</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E154" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -19602,10 +19602,10 @@
         <v>140</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E155" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -19613,10 +19613,10 @@
         <v>141</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E156" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -19624,10 +19624,10 @@
         <v>142</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E157" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
@@ -19635,10 +19635,10 @@
         <v>143</v>
       </c>
       <c r="B158" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E158" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -19646,10 +19646,10 @@
         <v>144</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E159" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -19657,10 +19657,10 @@
         <v>145</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E160" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -19668,10 +19668,10 @@
         <v>146</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E161" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -19679,10 +19679,10 @@
         <v>147</v>
       </c>
       <c r="B162" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E162" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
@@ -19690,10 +19690,10 @@
         <v>148</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E163" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -19701,10 +19701,10 @@
         <v>149</v>
       </c>
       <c r="B164" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E164" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
@@ -19712,12 +19712,12 @@
         <v>150</v>
       </c>
       <c r="B165" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added extra link for outcomes and comorbs from NPR in vardescription
</commit_message>
<xml_diff>
--- a/metadata/meta_variables.xlsx
+++ b/metadata/meta_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lina\STATISTIK\Projects\20200225_shfdb3\dm\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3FD08A-9508-4619-B0EB-AAA3CF36F7CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7730DE6C-3DB7-4A90-9B54-75BE03175DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32805" yWindow="2430" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -982,33 +982,18 @@
     <t xml:space="preserve">Max dose is different for different substances. Needs to be converted to % max dose or similar. </t>
   </si>
   <si>
-    <t>ICD-codes see https://kiheartfailure.github.io/shfdb3/</t>
-  </si>
-  <si>
     <t>Also see sos_durationhf</t>
   </si>
   <si>
-    <t>ICD-codes see https://kiheartfailure.github.io/shfdb3/. Also see shf_diabetes</t>
-  </si>
-  <si>
     <t>Also see sos_com_hypertension</t>
   </si>
   <si>
     <t>Also see sos_com_af</t>
   </si>
   <si>
-    <t>ICD-codes see https://kiheartfailure.github.io/shfdb3/. Also see shf_af</t>
-  </si>
-  <si>
-    <t>ICD-codes see https://kiheartfailure.github.io/shfdb3/. Also see shf_hypertension</t>
-  </si>
-  <si>
     <t>Also see sos_com_dcm</t>
   </si>
   <si>
-    <t>ICD-codes see https://kiheartfailure.github.io/shfdb3/. Also see shf_dcm</t>
-  </si>
-  <si>
     <t>2000-01-01 to 2010-04-08, 2017-04-27-</t>
   </si>
   <si>
@@ -1090,9 +1075,6 @@
     <t>Date of last follow-up/emigration/death/hf diagnosis (controls)</t>
   </si>
   <si>
-    <t>ICD-codes see https://kiheartfailure.github.io/shfdb3/. Time since hosp/visit (date of discharge (in-pat)/visit date (out-pat)) in any DIA position to shf_indexdtm. Note that dates in NPR and SwedeHF can differ slightly so caution should be used when looking at small durations. Also see shf_durationhf</t>
-  </si>
-  <si>
     <t>sos_prevhosphf</t>
   </si>
   <si>
@@ -1150,9 +1132,6 @@
     <t>shf_qol</t>
   </si>
   <si>
-    <t>ICD-codes see https://kiheartfailure.github.io/shfdb3/. Time since hosp (date of discharge) in any HDIA position to shf_indexdtm. Note that dates in NPR and SwedeHF can differ slightly so caution should be used when looking at small durations. If sos_location = "HF in-patient" it is set to 0</t>
-  </si>
-  <si>
     <t>shf_loopdiureticsub</t>
   </si>
   <si>
@@ -1166,6 +1145,27 @@
   </si>
   <si>
     <t>QoL EQ-5D</t>
+  </si>
+  <si>
+    <t>ICD-codes see https://kiheartfailure.github.io/shfdb3/construction/dm/#comorbidities-and-outcomes-from-npr. Time since hosp/visit (date of discharge (in-pat)/visit date (out-pat)) in any DIA position to shf_indexdtm. Note that dates in NPR and SwedeHF can differ slightly so caution should be used when looking at small durations. Also see shf_durationhf</t>
+  </si>
+  <si>
+    <t>ICD-codes see https://kiheartfailure.github.io/shfdb3/construction/dm/#comorbidities-and-outcomes-from-npr. Time since hosp (date of discharge) in any HDIA position to shf_indexdtm. Note that dates in NPR and SwedeHF can differ slightly so caution should be used when looking at small durations. If sos_location = "HF in-patient" it is set to 0</t>
+  </si>
+  <si>
+    <t>ICD-codes see https://kiheartfailure.github.io/shfdb3/construction/dm/#comorbidities-and-outcomes-from-npr. Also see shf_hypertension</t>
+  </si>
+  <si>
+    <t>ICD-codes see https://kiheartfailure.github.io/shfdb3/construction/dm/#comorbidities-and-outcomes-from-npr. Also see shf_diabetes</t>
+  </si>
+  <si>
+    <t>ICD-codes see https://kiheartfailure.github.io/shfdb3/construction/dm/#comorbidities-and-outcomes-from-npr</t>
+  </si>
+  <si>
+    <t>ICD-codes see https://kiheartfailure.github.io/shfdb3/construction/dm/#comorbidities-and-outcomes-from-npr. Also see shf_dcm</t>
+  </si>
+  <si>
+    <t>ICD-codes see https://kiheartfailure.github.io/shfdb3/construction/dm/#comorbidities-and-outcomes-from-npr. Also see shf_af</t>
   </si>
 </sst>
 </file>
@@ -1545,8 +1545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1629,13 +1629,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1668,7 +1668,7 @@
         <v>294</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1682,12 +1682,12 @@
         <v>202</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>201</v>
@@ -1696,10 +1696,10 @@
         <v>202</v>
       </c>
       <c r="D13" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>337</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1740,7 +1740,7 @@
         <v>283</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1751,31 +1751,31 @@
         <v>196</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1794,10 +1794,10 @@
         <v>199</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1841,7 +1841,7 @@
         <v>209</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1907,7 +1907,7 @@
         <v>207</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1918,7 +1918,7 @@
         <v>158</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>312</v>
@@ -1941,7 +1941,7 @@
         <v>30</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>296</v>
@@ -1949,7 +1949,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>165</v>
@@ -2044,10 +2044,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -2167,7 +2167,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>180</v>
@@ -2219,7 +2219,7 @@
         <v>184</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -2233,7 +2233,7 @@
         <v>313</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="E62" s="4" t="s">
         <v>319</v>
@@ -2252,7 +2252,7 @@
         <v>52</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -2260,7 +2260,7 @@
         <v>53</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="E65" s="4" t="s">
         <v>318</v>
@@ -2343,7 +2343,7 @@
         <v>223</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="E72" s="4" t="s">
         <v>218</v>
@@ -2357,24 +2357,24 @@
         <v>189</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>189</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -2385,10 +2385,10 @@
         <v>190</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -2399,10 +2399,10 @@
         <v>224</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -2413,7 +2413,7 @@
         <v>225</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -2424,7 +2424,7 @@
         <v>226</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -2435,10 +2435,10 @@
         <v>227</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -2449,10 +2449,10 @@
         <v>191</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -2463,10 +2463,10 @@
         <v>220</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -2498,10 +2498,10 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -2515,12 +2515,12 @@
         <v>297</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="B87" s="4" t="s">
         <v>162</v>
@@ -2529,7 +2529,7 @@
         <v>297</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -2545,7 +2545,7 @@
         <v>72</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="E89" s="4" t="s">
         <v>314</v>
@@ -2613,10 +2613,10 @@
     </row>
     <row r="96" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -2627,21 +2627,21 @@
         <v>199</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>356</v>
+        <v>375</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="E98" s="4" t="s">
         <v>376</v>
@@ -2649,13 +2649,13 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="B99" s="4" t="s">
         <v>196</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -2666,7 +2666,7 @@
         <v>190</v>
       </c>
       <c r="E100" s="4" t="s">
-        <v>326</v>
+        <v>377</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2677,7 +2677,7 @@
         <v>189</v>
       </c>
       <c r="E101" s="4" t="s">
-        <v>322</v>
+        <v>378</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -2688,7 +2688,7 @@
         <v>235</v>
       </c>
       <c r="E102" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -2699,7 +2699,7 @@
         <v>236</v>
       </c>
       <c r="E103" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -2710,7 +2710,7 @@
         <v>237</v>
       </c>
       <c r="E104" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -2721,7 +2721,7 @@
         <v>238</v>
       </c>
       <c r="E105" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -2732,7 +2732,7 @@
         <v>239</v>
       </c>
       <c r="E106" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -2743,7 +2743,7 @@
         <v>227</v>
       </c>
       <c r="E107" s="4" t="s">
-        <v>328</v>
+        <v>380</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -2754,7 +2754,7 @@
         <v>240</v>
       </c>
       <c r="E108" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -2765,7 +2765,7 @@
         <v>224</v>
       </c>
       <c r="E109" s="4" t="s">
-        <v>325</v>
+        <v>381</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -2776,7 +2776,7 @@
         <v>241</v>
       </c>
       <c r="E110" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -2787,7 +2787,7 @@
         <v>242</v>
       </c>
       <c r="E111" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -2798,7 +2798,7 @@
         <v>243</v>
       </c>
       <c r="E112" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -2809,7 +2809,7 @@
         <v>244</v>
       </c>
       <c r="E113" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -2817,10 +2817,10 @@
         <v>94</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="E114" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -2831,7 +2831,7 @@
         <v>245</v>
       </c>
       <c r="E115" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -2842,7 +2842,7 @@
         <v>246</v>
       </c>
       <c r="E116" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -2853,7 +2853,7 @@
         <v>247</v>
       </c>
       <c r="E117" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -2864,7 +2864,7 @@
         <v>248</v>
       </c>
       <c r="E118" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -2875,7 +2875,7 @@
         <v>249</v>
       </c>
       <c r="E119" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -2883,10 +2883,10 @@
         <v>100</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="E120" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -2897,7 +2897,7 @@
         <v>250</v>
       </c>
       <c r="E121" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -2908,7 +2908,7 @@
         <v>251</v>
       </c>
       <c r="E122" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -2919,7 +2919,7 @@
         <v>252</v>
       </c>
       <c r="E123" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
@@ -2930,7 +2930,7 @@
         <v>253</v>
       </c>
       <c r="E124" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
@@ -2941,7 +2941,7 @@
         <v>254</v>
       </c>
       <c r="E125" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -2952,7 +2952,7 @@
         <v>255</v>
       </c>
       <c r="E126" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -2963,7 +2963,7 @@
         <v>257</v>
       </c>
       <c r="E127" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -2974,7 +2974,7 @@
         <v>258</v>
       </c>
       <c r="E128" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -2982,21 +2982,21 @@
         <v>109</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="E129" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="E130" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -3007,7 +3007,7 @@
         <v>259</v>
       </c>
       <c r="E131" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -3015,10 +3015,10 @@
         <v>111</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="E132" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -3029,7 +3029,7 @@
         <v>261</v>
       </c>
       <c r="E133" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -3037,10 +3037,10 @@
         <v>113</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="E134" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -3051,7 +3051,7 @@
         <v>262</v>
       </c>
       <c r="E135" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -3059,10 +3059,10 @@
         <v>115</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="E136" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -3073,7 +3073,7 @@
         <v>263</v>
       </c>
       <c r="E137" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -3081,10 +3081,10 @@
         <v>117</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="E138" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -3095,7 +3095,7 @@
         <v>264</v>
       </c>
       <c r="E139" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -3103,10 +3103,10 @@
         <v>119</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="E140" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -3117,7 +3117,7 @@
         <v>265</v>
       </c>
       <c r="E141" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -3125,10 +3125,10 @@
         <v>121</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="E142" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -3139,7 +3139,7 @@
         <v>266</v>
       </c>
       <c r="E143" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -3147,10 +3147,10 @@
         <v>123</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="E144" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -3158,10 +3158,10 @@
         <v>124</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="E145" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -3172,7 +3172,7 @@
         <v>267</v>
       </c>
       <c r="E146" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -3180,10 +3180,10 @@
         <v>126</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="E147" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
@@ -3194,7 +3194,7 @@
         <v>260</v>
       </c>
       <c r="E148" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -3202,10 +3202,10 @@
         <v>128</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="E149" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
@@ -3216,7 +3216,7 @@
         <v>268</v>
       </c>
       <c r="E150" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -3224,10 +3224,10 @@
         <v>130</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="E151" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -3238,7 +3238,7 @@
         <v>270</v>
       </c>
       <c r="E152" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -3246,10 +3246,10 @@
         <v>132</v>
       </c>
       <c r="C153" s="4" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="E153" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -3260,7 +3260,7 @@
         <v>269</v>
       </c>
       <c r="E154" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -3268,10 +3268,10 @@
         <v>134</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="E155" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -3282,7 +3282,7 @@
         <v>272</v>
       </c>
       <c r="E156" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -3290,10 +3290,10 @@
         <v>136</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="E157" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
@@ -3304,7 +3304,7 @@
         <v>273</v>
       </c>
       <c r="E158" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -3312,10 +3312,10 @@
         <v>138</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="E159" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -3326,7 +3326,7 @@
         <v>274</v>
       </c>
       <c r="E160" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -3334,10 +3334,10 @@
         <v>140</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="E161" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -3348,7 +3348,7 @@
         <v>275</v>
       </c>
       <c r="E162" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
@@ -3356,10 +3356,10 @@
         <v>142</v>
       </c>
       <c r="C163" s="4" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="E163" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -3370,7 +3370,7 @@
         <v>276</v>
       </c>
       <c r="E164" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
@@ -3378,10 +3378,10 @@
         <v>144</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="E165" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
@@ -3392,7 +3392,7 @@
         <v>271</v>
       </c>
       <c r="E166" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -3400,10 +3400,10 @@
         <v>146</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="E167" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
@@ -3414,7 +3414,7 @@
         <v>277</v>
       </c>
       <c r="E168" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
@@ -3425,7 +3425,7 @@
         <v>278</v>
       </c>
       <c r="E169" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
@@ -3436,7 +3436,7 @@
         <v>256</v>
       </c>
       <c r="E170" s="4" t="s">
-        <v>320</v>
+        <v>379</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>